<commit_message>
Update Gantt chart & some docs
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thao My\Software_tech_assignment\2810ICT-Assignment-Group55\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thao My\2810ICT_Assignment_Group55\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95C5C2E-CF06-4511-BFA4-A5257B4414C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E9F8F2-7579-44EC-B6CC-9576BCBAEDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -573,7 +573,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -643,6 +643,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
@@ -654,51 +696,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1102,8 +1099,8 @@
   </sheetPr>
   <dimension ref="B1:BO35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="40" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="60" zoomScaleNormal="40" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.796875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -1133,13 +1130,13 @@
       <c r="G1" s="12"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1147,37 +1144,37 @@
         <v>32</v>
       </c>
       <c r="J2" s="15"/>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="32"/>
       <c r="P2" s="16"/>
-      <c r="Q2" s="29" t="s">
+      <c r="Q2" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="31"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="32"/>
       <c r="U2" s="17"/>
-      <c r="V2" s="33" t="s">
+      <c r="V2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="34"/>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="36"/>
       <c r="Z2" s="18"/>
-      <c r="AA2" s="33" t="s">
+      <c r="AA2" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="34"/>
-      <c r="AC2" s="34"/>
-      <c r="AD2" s="34"/>
-      <c r="AE2" s="34"/>
-      <c r="AF2" s="34"/>
-      <c r="AG2" s="35"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="36"/>
       <c r="AH2" s="19"/>
       <c r="AI2" s="21" t="s">
         <v>4</v>
@@ -1191,19 +1188,19 @@
       <c r="AP2" s="22"/>
     </row>
     <row r="3" spans="2:67" s="11" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="26" t="s">
+      <c r="B3" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="40" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="28" t="s">
@@ -1233,12 +1230,12 @@
       <c r="AA3" s="10"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="25"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1429,22 +1426,21 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="8"/>
-      <c r="H5" s="39"/>
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="40">
-        <v>1</v>
-      </c>
-      <c r="D6" s="40">
+      <c r="C6" s="26">
+        <v>1</v>
+      </c>
+      <c r="D6" s="26">
         <v>5</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E6" s="26">
         <v>2</v>
       </c>
-      <c r="F6" s="40">
+      <c r="F6" s="26">
         <v>7</v>
       </c>
       <c r="G6" s="8">
@@ -1452,19 +1448,19 @@
       </c>
     </row>
     <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="40">
+      <c r="C7" s="26">
         <v>2</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="26">
         <v>10</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="26">
         <v>3</v>
       </c>
-      <c r="F7" s="40">
+      <c r="F7" s="26">
         <v>9</v>
       </c>
       <c r="G7" s="8">
@@ -1472,19 +1468,19 @@
       </c>
     </row>
     <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="40">
+      <c r="C8" s="26">
         <v>3</v>
       </c>
-      <c r="D8" s="40">
+      <c r="D8" s="26">
         <v>4</v>
       </c>
-      <c r="E8" s="40">
+      <c r="E8" s="26">
         <v>3</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="26">
         <v>6</v>
       </c>
       <c r="G8" s="8">
@@ -1492,19 +1488,19 @@
       </c>
     </row>
     <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="40">
+      <c r="C9" s="26">
         <v>10</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="26">
         <v>7</v>
       </c>
-      <c r="E9" s="40">
+      <c r="E9" s="26">
         <v>12</v>
       </c>
-      <c r="F9" s="40">
+      <c r="F9" s="26">
         <v>7</v>
       </c>
       <c r="G9" s="8">
@@ -1512,7 +1508,7 @@
       </c>
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="25" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="7"/>
@@ -1522,7 +1518,7 @@
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="23" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="7"/>
@@ -1532,19 +1528,19 @@
       <c r="G11" s="8"/>
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="40">
+      <c r="C12" s="26">
         <v>13</v>
       </c>
-      <c r="D12" s="40">
+      <c r="D12" s="26">
         <v>7</v>
       </c>
-      <c r="E12" s="40">
+      <c r="E12" s="26">
         <v>13</v>
       </c>
-      <c r="F12" s="40">
+      <c r="F12" s="26">
         <v>8</v>
       </c>
       <c r="G12" s="8">
@@ -1552,19 +1548,19 @@
       </c>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="40">
+      <c r="C13" s="26">
         <v>13</v>
       </c>
-      <c r="D13" s="40">
+      <c r="D13" s="26">
         <v>7</v>
       </c>
-      <c r="E13" s="40">
+      <c r="E13" s="26">
         <v>13</v>
       </c>
-      <c r="F13" s="40">
+      <c r="F13" s="26">
         <v>6</v>
       </c>
       <c r="G13" s="8">
@@ -1582,19 +1578,19 @@
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="41">
+      <c r="C15" s="27">
         <v>14</v>
       </c>
-      <c r="D15" s="40">
+      <c r="D15" s="26">
         <v>6</v>
       </c>
-      <c r="E15" s="40">
+      <c r="E15" s="26">
         <v>15</v>
       </c>
-      <c r="F15" s="40">
+      <c r="F15" s="26">
         <v>5</v>
       </c>
       <c r="G15" s="8">
@@ -1602,19 +1598,19 @@
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="40">
+      <c r="C16" s="26">
         <v>16</v>
       </c>
-      <c r="D16" s="40">
+      <c r="D16" s="26">
         <v>5</v>
       </c>
-      <c r="E16" s="40">
+      <c r="E16" s="26">
         <v>16</v>
       </c>
-      <c r="F16" s="40">
+      <c r="F16" s="26">
         <v>5</v>
       </c>
       <c r="G16" s="8">
@@ -1622,19 +1618,19 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="40">
+      <c r="C17" s="26">
         <v>17</v>
       </c>
-      <c r="D17" s="40">
+      <c r="D17" s="26">
         <v>6</v>
       </c>
-      <c r="E17" s="40">
+      <c r="E17" s="26">
         <v>17</v>
       </c>
-      <c r="F17" s="40">
+      <c r="F17" s="26">
         <v>7</v>
       </c>
       <c r="G17" s="8">
@@ -1642,19 +1638,19 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="40">
+      <c r="C18" s="26">
         <v>19</v>
       </c>
-      <c r="D18" s="40">
+      <c r="D18" s="26">
         <v>11</v>
       </c>
-      <c r="E18" s="40">
+      <c r="E18" s="26">
         <v>20</v>
       </c>
-      <c r="F18" s="40">
+      <c r="F18" s="26">
         <v>12</v>
       </c>
       <c r="G18" s="8">
@@ -1662,19 +1658,19 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="40">
+      <c r="C19" s="26">
         <v>22</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="26">
         <v>10</v>
       </c>
-      <c r="E19" s="40">
+      <c r="E19" s="26">
         <v>23</v>
       </c>
-      <c r="F19" s="40">
+      <c r="F19" s="26">
         <v>10</v>
       </c>
       <c r="G19" s="8">
@@ -1682,7 +1678,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="25" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="7"/>
@@ -1692,7 +1688,7 @@
       <c r="G20" s="8"/>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="23" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="7"/>
@@ -1702,51 +1698,63 @@
       <c r="G21" s="8"/>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="40">
+      <c r="C22" s="26">
         <v>33</v>
       </c>
-      <c r="D22" s="40">
+      <c r="D22" s="26">
         <v>5</v>
       </c>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
+      <c r="E22" s="26">
+        <v>37</v>
+      </c>
+      <c r="F22" s="26">
+        <v>6</v>
+      </c>
       <c r="G22" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="40">
+      <c r="C23" s="26">
         <v>37</v>
       </c>
-      <c r="D23" s="40">
+      <c r="D23" s="26">
         <v>3</v>
       </c>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
+      <c r="E23" s="26">
+        <v>40</v>
+      </c>
+      <c r="F23" s="26">
+        <v>3</v>
+      </c>
       <c r="G23" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="40">
+      <c r="C24" s="26">
         <v>38</v>
       </c>
-      <c r="D24" s="40">
+      <c r="D24" s="26">
         <v>6</v>
       </c>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
+      <c r="E24" s="26">
+        <v>41</v>
+      </c>
+      <c r="F24" s="26">
+        <v>6</v>
+      </c>
       <c r="G24" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
@@ -1760,51 +1768,63 @@
       <c r="G25" s="8"/>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="40">
+      <c r="C26" s="26">
         <v>38</v>
       </c>
-      <c r="D26" s="40">
+      <c r="D26" s="26">
         <v>10</v>
       </c>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
+      <c r="E26" s="26">
+        <v>36</v>
+      </c>
+      <c r="F26" s="26">
+        <v>12</v>
+      </c>
       <c r="G26" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="40">
+      <c r="C27" s="26">
         <v>42</v>
       </c>
-      <c r="D27" s="40">
+      <c r="D27" s="26">
         <v>6</v>
       </c>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
+      <c r="E27" s="26">
+        <v>43</v>
+      </c>
+      <c r="F27" s="26">
+        <v>6</v>
+      </c>
       <c r="G27" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="40">
+      <c r="C28" s="26">
         <v>46</v>
       </c>
-      <c r="D28" s="40">
+      <c r="D28" s="26">
         <v>5</v>
       </c>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40"/>
+      <c r="E28" s="26">
+        <v>46</v>
+      </c>
+      <c r="F28" s="26">
+        <v>5</v>
+      </c>
       <c r="G28" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
@@ -1817,14 +1837,18 @@
       <c r="D29" s="7">
         <v>11</v>
       </c>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+      <c r="E29" s="7">
+        <v>51</v>
+      </c>
+      <c r="F29" s="7">
+        <v>10</v>
+      </c>
       <c r="G29" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="25" t="s">
         <v>39</v>
       </c>
       <c r="C30" s="7"/>
@@ -1834,39 +1858,47 @@
       <c r="G30" s="8"/>
     </row>
     <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="40">
-        <v>1</v>
-      </c>
-      <c r="D31" s="40">
+      <c r="C31" s="26">
+        <v>1</v>
+      </c>
+      <c r="D31" s="26">
         <v>60</v>
       </c>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
+      <c r="E31" s="26">
+        <v>5</v>
+      </c>
+      <c r="F31" s="26">
+        <v>56</v>
+      </c>
       <c r="G31" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="40">
+      <c r="C32" s="26">
         <v>43</v>
       </c>
-      <c r="D32" s="40">
+      <c r="D32" s="26">
         <v>18</v>
       </c>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
+      <c r="E32" s="26">
+        <v>45</v>
+      </c>
+      <c r="F32" s="26">
+        <v>16</v>
+      </c>
       <c r="G32" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="25" t="s">
         <v>41</v>
       </c>
       <c r="C33" s="7"/>
@@ -1876,50 +1908,58 @@
       <c r="G33" s="8"/>
     </row>
     <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="40">
+      <c r="C34" s="26">
         <v>52</v>
       </c>
-      <c r="D34" s="40">
+      <c r="D34" s="26">
         <v>3</v>
       </c>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
+      <c r="E34" s="26">
+        <v>55</v>
+      </c>
+      <c r="F34" s="26">
+        <v>3</v>
+      </c>
       <c r="G34" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="40">
+      <c r="C35" s="26">
         <v>52</v>
       </c>
-      <c r="D35" s="40">
+      <c r="D35" s="26">
         <v>9</v>
       </c>
-      <c r="E35" s="40"/>
-      <c r="F35" s="40"/>
+      <c r="E35" s="26">
+        <v>55</v>
+      </c>
+      <c r="F35" s="26">
+        <v>6</v>
+      </c>
       <c r="G35" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BO4">
     <cfRule type="expression" dxfId="8" priority="8">
@@ -1984,4 +2024,10 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{c9f92db8-2851-4df9-9d12-fab52f5b1415}" enabled="1" method="Standard" siteId="{5a7cc8ab-a4dc-4f9b-bf60-66714049ad62}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Updating project plan and Gantt chart
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thao My\2810ICT_Assignment_Group55\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E9F8F2-7579-44EC-B6CC-9576BCBAEDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F0237F-B9D5-4129-8351-6F7568A96664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -658,12 +658,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -684,18 +696,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1099,8 +1099,8 @@
   </sheetPr>
   <dimension ref="B1:BO35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="60" zoomScaleNormal="40" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="54" zoomScaleNormal="40" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="BR10" sqref="BR10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.796875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -1130,13 +1130,13 @@
       <c r="G1" s="12"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1144,37 +1144,37 @@
         <v>32</v>
       </c>
       <c r="J2" s="15"/>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="32"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="36"/>
       <c r="P2" s="16"/>
-      <c r="Q2" s="30" t="s">
+      <c r="Q2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="32"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="36"/>
       <c r="U2" s="17"/>
-      <c r="V2" s="34" t="s">
+      <c r="V2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="36"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="40"/>
       <c r="Z2" s="18"/>
-      <c r="AA2" s="34" t="s">
+      <c r="AA2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="35"/>
-      <c r="AC2" s="35"/>
-      <c r="AD2" s="35"/>
-      <c r="AE2" s="35"/>
-      <c r="AF2" s="35"/>
-      <c r="AG2" s="36"/>
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39"/>
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
+      <c r="AG2" s="40"/>
       <c r="AH2" s="19"/>
       <c r="AI2" s="21" t="s">
         <v>4</v>
@@ -1188,22 +1188,22 @@
       <c r="AP2" s="22"/>
     </row>
     <row r="3" spans="2:67" s="11" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="40" t="s">
+      <c r="B3" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="33" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="20" t="s">
@@ -1230,12 +1230,12 @@
       <c r="AA3" s="10"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="39"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1888,10 +1888,10 @@
         <v>18</v>
       </c>
       <c r="E32" s="26">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F32" s="26">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G32" s="8">
         <v>1</v>
@@ -1921,7 +1921,7 @@
         <v>55</v>
       </c>
       <c r="F34" s="26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G34" s="8">
         <v>1</v>
@@ -1938,10 +1938,10 @@
         <v>9</v>
       </c>
       <c r="E35" s="26">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F35" s="26">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G35" s="8">
         <v>1</v>
@@ -1949,17 +1949,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BO4">
     <cfRule type="expression" dxfId="8" priority="8">

</xml_diff>